<commit_message>
update them phan lien tuc
</commit_message>
<xml_diff>
--- a/data/quan_sat.xlsx
+++ b/data/quan_sat.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:BM4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,22 +485,166 @@
       <c r="Q1" s="1" t="n">
         <v>16</v>
       </c>
+      <c r="R1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="1" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
       <c r="C2" t="n">
         <v>3</v>
       </c>
-      <c r="D2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
-        <v>6</v>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
         <v>7</v>
       </c>
@@ -508,136 +652,440 @@
       <c r="I2" t="n">
         <v>9</v>
       </c>
-      <c r="J2" t="n">
-        <v>10</v>
-      </c>
-      <c r="K2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="n">
+        <v>11</v>
+      </c>
       <c r="L2" t="n">
         <v>12</v>
       </c>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="n">
+        <v>14</v>
+      </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="n">
+        <v>19</v>
+      </c>
+      <c r="T2" t="n">
+        <v>20</v>
+      </c>
+      <c r="U2" t="n">
+        <v>21</v>
+      </c>
+      <c r="V2" t="n">
+        <v>22</v>
+      </c>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="n">
+        <v>24</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="n">
+        <v>27</v>
+      </c>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="n">
+        <v>31</v>
+      </c>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="n">
+        <v>33</v>
+      </c>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="n">
+        <v>35</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="n">
+        <v>41</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>42</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>43</v>
+      </c>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="n">
+        <v>45</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>46</v>
+      </c>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="n">
+        <v>48</v>
+      </c>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="n">
+        <v>52</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>53</v>
+      </c>
+      <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="n">
+        <v>55</v>
+      </c>
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="n">
+        <v>57</v>
+      </c>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr"/>
+      <c r="BH2" t="n">
+        <v>60</v>
+      </c>
+      <c r="BI2" t="inlineStr"/>
+      <c r="BJ2" t="n">
+        <v>62</v>
+      </c>
+      <c r="BK2" t="inlineStr"/>
+      <c r="BL2" t="inlineStr"/>
+      <c r="BM2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr"/>
+        <v>18</v>
+      </c>
+      <c r="B3" t="n">
+        <v>17</v>
+      </c>
       <c r="C3" t="n">
-        <v>16</v>
-      </c>
-      <c r="D3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>15</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>8</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
-        <v>14</v>
-      </c>
-      <c r="J3" t="n">
-        <v>11</v>
-      </c>
-      <c r="K3" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>16</v>
+      </c>
       <c r="L3" t="n">
         <v>13</v>
       </c>
       <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="n">
+        <v>15</v>
+      </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="n">
+        <v>40</v>
+      </c>
+      <c r="T3" t="n">
+        <v>39</v>
+      </c>
+      <c r="U3" t="n">
+        <v>30</v>
+      </c>
+      <c r="V3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>26</v>
+      </c>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="n">
+        <v>32</v>
+      </c>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="n">
+        <v>34</v>
+      </c>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="n">
+        <v>38</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>37</v>
+      </c>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="n">
+        <v>64</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>51</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>44</v>
+      </c>
+      <c r="AR3" t="inlineStr"/>
+      <c r="AS3" t="n">
+        <v>50</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>47</v>
+      </c>
+      <c r="AU3" t="inlineStr"/>
+      <c r="AV3" t="n">
+        <v>49</v>
+      </c>
+      <c r="AW3" t="inlineStr"/>
+      <c r="AX3" t="inlineStr"/>
+      <c r="AY3" t="inlineStr"/>
+      <c r="AZ3" t="n">
+        <v>59</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>54</v>
+      </c>
+      <c r="BB3" t="inlineStr"/>
+      <c r="BC3" t="n">
+        <v>56</v>
+      </c>
+      <c r="BD3" t="inlineStr"/>
+      <c r="BE3" t="n">
+        <v>58</v>
+      </c>
+      <c r="BF3" t="inlineStr"/>
+      <c r="BG3" t="inlineStr"/>
+      <c r="BH3" t="n">
+        <v>61</v>
+      </c>
+      <c r="BI3" t="inlineStr"/>
+      <c r="BJ3" t="n">
+        <v>63</v>
+      </c>
+      <c r="BK3" t="inlineStr"/>
+      <c r="BL3" t="inlineStr"/>
+      <c r="BM3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">| 60.78 Co | 39.22 Khong | </t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
         <is>
           <t>Co</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">| 35.48 Co | 64.52 Khong | </t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">| 68.75 Co | 31.25 Khong | </t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
         <is>
           <t>Co</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">| 55.56 Khong | 44.44 Co | </t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">| 42.86 Khong | 57.14 Co | </t>
-        </is>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
+          <t>ko bt</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>Co</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">| 60.0 Khong | 40.0 Co | </t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">| 33.33 Khong | 66.67 Co | </t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
         <is>
           <t>ko bt</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">| 33.33 Khong | 66.67 Co | </t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Khong</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
         <is>
           <t>Co</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Khong</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Khong</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>Khong</t>
-        </is>
-      </c>
       <c r="Q4" t="inlineStr">
+        <is>
+          <t>ko bt</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>ko bt</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Khong</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>ko bt</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>ko bt</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>ko bt</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>Khong</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Co</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>Co</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>Co</t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>Khong</t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr">
+        <is>
+          <t>Khong</t>
+        </is>
+      </c>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t>Khong</t>
+        </is>
+      </c>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr">
+        <is>
+          <t>Khong</t>
+        </is>
+      </c>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t>ko bt</t>
+        </is>
+      </c>
+      <c r="AV4" t="inlineStr"/>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t>Co</t>
+        </is>
+      </c>
+      <c r="AX4" t="inlineStr">
+        <is>
+          <t>Khong</t>
+        </is>
+      </c>
+      <c r="AY4" t="inlineStr">
+        <is>
+          <t>Khong</t>
+        </is>
+      </c>
+      <c r="AZ4" t="inlineStr"/>
+      <c r="BA4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr">
+        <is>
+          <t>ko bt</t>
+        </is>
+      </c>
+      <c r="BC4" t="inlineStr"/>
+      <c r="BD4" t="inlineStr">
+        <is>
+          <t>Co</t>
+        </is>
+      </c>
+      <c r="BE4" t="inlineStr"/>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>Khong</t>
+        </is>
+      </c>
+      <c r="BG4" t="inlineStr">
+        <is>
+          <t>Co</t>
+        </is>
+      </c>
+      <c r="BH4" t="inlineStr"/>
+      <c r="BI4" t="inlineStr">
+        <is>
+          <t>Khong</t>
+        </is>
+      </c>
+      <c r="BJ4" t="inlineStr"/>
+      <c r="BK4" t="inlineStr">
+        <is>
+          <t>Co</t>
+        </is>
+      </c>
+      <c r="BL4" t="inlineStr">
+        <is>
+          <t>Khong</t>
+        </is>
+      </c>
+      <c r="BM4" t="inlineStr">
         <is>
           <t>Khong</t>
         </is>

</xml_diff>